<commit_message>
Alterations for model performance figure
</commit_message>
<xml_diff>
--- a/Results_Figure/Results.xlsx
+++ b/Results_Figure/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conve\Dropbox\C_Projects - Current - Lead\Seaducks\Seaduck Detection Project\seaduck_detection\Results_Figure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suchabingly/Documents/Windsor/UW Postdoc/Sea duck detection/seaduck_detection/Results_Figure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8717CD2-FC1D-4DDD-89A0-97276D419AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AE73E6-F803-6C4F-A44A-E9CBF9F852E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" activeTab="1" xr2:uid="{B8D3EF7E-0C74-4076-9E27-C28430A5E0B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23660" windowHeight="15240" xr2:uid="{B8D3EF7E-0C74-4076-9E27-C28430A5E0B4}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -1072,17 +1072,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B725F6A2-44FE-4A8D-B84E-DE81585CF7D3}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.84375" customWidth="1"/>
-    <col min="2" max="7" width="31.84375" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="7" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1128,7 +1129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1220,7 +1221,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
@@ -1266,7 +1267,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>67</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>74</v>
       </c>
@@ -1358,7 +1359,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>80</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>86</v>
       </c>
@@ -1404,7 +1405,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>92</v>
       </c>
@@ -1427,7 +1428,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>105</v>
       </c>
@@ -1473,7 +1474,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>111</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>117</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>123</v>
       </c>
@@ -1542,7 +1543,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>129</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>135</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>141</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>147</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>153</v>
       </c>
@@ -1657,7 +1658,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>159</v>
       </c>
@@ -1680,7 +1681,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>165</v>
       </c>
@@ -1703,7 +1704,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>171</v>
       </c>
@@ -1726,7 +1727,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>177</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>183</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>189</v>
       </c>
@@ -1791,7 +1792,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>190</v>
       </c>
@@ -1810,7 +1811,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>191</v>
       </c>
@@ -1829,7 +1830,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>192</v>
       </c>
@@ -1848,7 +1849,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>193</v>
       </c>
@@ -1867,7 +1868,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
     </row>
-    <row r="36" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>194</v>
       </c>
@@ -1886,7 +1887,7 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>195</v>
       </c>
@@ -1905,7 +1906,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>196</v>
       </c>
@@ -1924,7 +1925,7 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
-    <row r="39" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>197</v>
       </c>
@@ -1943,7 +1944,7 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
     </row>
-    <row r="40" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>198</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>204</v>
       </c>
@@ -1999,18 +2000,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5E0983-42DE-4571-9D68-BDAAC40F44EE}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="23.53515625" customWidth="1"/>
-    <col min="3" max="5" width="12.4609375" customWidth="1"/>
-    <col min="6" max="11" width="12.23046875" customWidth="1"/>
+    <col min="1" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="11" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2045,7 +2046,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>215</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>35</v>
       </c>
@@ -2150,7 +2151,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>54</v>
       </c>
@@ -2220,7 +2221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>105</v>
       </c>
@@ -2290,7 +2291,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>147</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>183</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>204</v>
       </c>

</xml_diff>